<commit_message>
in-game questions, measures with experience and income distribution table
</commit_message>
<xml_diff>
--- a/Datasets/vjcortesa_Presurvey_questions overview.xlsx
+++ b/Datasets/vjcortesa_Presurvey_questions overview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/jcortesarevalo_tudelft_nl/Documents/Documents/TUDelft/18_Game Data Analysis/R data analysis BEPs/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1117" documentId="11_F25DC773A252ABDACC10482FB9DB7A865ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B5BEA3A-2316-43D3-997C-D36CCE88438C}"/>
+  <xr:revisionPtr revIDLastSave="1121" documentId="11_F25DC773A252ABDACC10482FB9DB7A865ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDD39810-E8D1-40CA-A252-7B7B124F1C24}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="232">
   <si>
     <t>session_19_250923_EPA_IntroDays_Overasselt</t>
   </si>
@@ -733,6 +733,9 @@
   </si>
   <si>
     <t>Q_Role_Faculty_Other</t>
+  </si>
+  <si>
+    <t>RiskPerception_6</t>
   </si>
 </sst>
 </file>
@@ -761,7 +764,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -786,6 +789,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -799,7 +808,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -827,6 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,8 +1120,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1516,6 +1526,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>231</v>
+      </c>
       <c r="B23" t="s">
         <v>98</v>
       </c>
@@ -1742,8 +1755,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2374,9 +2387,9 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" t="str">
         <f>+Overview!A23</f>
-        <v>0</v>
+        <v>RiskPerception_6</v>
       </c>
       <c r="B19" t="str">
         <f>+Overview!B23</f>
@@ -3472,9 +3485,9 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" t="str">
         <f>+Overview!A23</f>
-        <v>0</v>
+        <v>RiskPerception_6</v>
       </c>
       <c r="B19" t="str">
         <f>+Overview!B23</f>
@@ -3904,8 +3917,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4488,9 +4501,9 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" t="str">
         <f>+Overview!A23</f>
-        <v>0</v>
+        <v>RiskPerception_6</v>
       </c>
       <c r="B19" t="str">
         <f>+Overview!B23</f>

</xml_diff>